<commit_message>
Update 10-8-2025 Nyotengu Sprite
</commit_message>
<xml_diff>
--- a/Waimonlist.xlsx
+++ b/Waimonlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NUTTOD\Develope\ROMHACK\ROM\WAIMON\Gitupload\Waimon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57747F7A-C013-4321-9F9E-4D21F3EA2CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9F5DA9-93DA-4CF4-AC5E-9D00710669B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5352" yWindow="1620" windowWidth="17280" windowHeight="11268" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5784" yWindow="108" windowWidth="16008" windowHeight="11472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2009,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F387"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
+      <selection activeCell="E257" sqref="E257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>